<commit_message>
Make works with libraries.
</commit_message>
<xml_diff>
--- a/Wiring/RCCar Wiring.xlsx
+++ b/Wiring/RCCar Wiring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephhellerstein/home/Technical/Arduino/RCCar/Wiring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F62E8A-6F53-AF4F-910C-E09C9447F7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D12729-C870-6242-99D0-EF33AFC56F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16620" yWindow="1140" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{0BE17797-1956-CB45-AFDB-7B911D2BE600}"/>
+    <workbookView xWindow="7800" yWindow="1140" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{0BE17797-1956-CB45-AFDB-7B911D2BE600}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="63">
   <si>
     <t>Arduino 2560</t>
   </si>
@@ -200,13 +200,40 @@
   </si>
   <si>
     <t>BACK MOTOR DRIVER</t>
+  </si>
+  <si>
+    <t>US-Front</t>
+  </si>
+  <si>
+    <t>US-Back</t>
+  </si>
+  <si>
+    <t>Vcc</t>
+  </si>
+  <si>
+    <t>Trig</t>
+  </si>
+  <si>
+    <t>Echo</t>
+  </si>
+  <si>
+    <t>Gnd</t>
+  </si>
+  <si>
+    <t>US-Left</t>
+  </si>
+  <si>
+    <t>US-Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  5+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -279,6 +306,14 @@
       <b/>
       <sz val="18"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -388,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -419,6 +454,9 @@
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,10 +774,10 @@
   <dimension ref="A1:AG22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1022,7 +1060,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1366,7 +1404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700F51A8-449D-DA44-88E3-D7CBBE9512A0}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1727,12 +1765,155 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D2A009-778F-3F4C-8093-CF2587473A17}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="O12" sqref="O12:P13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" s="30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="Q5" s="4"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="G6" s="31"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>13</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>22</v>
+      </c>
+      <c r="C8" s="31"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>23</v>
+      </c>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>34</v>
+      </c>
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>35</v>
+      </c>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>36</v>
+      </c>
+      <c r="O12" s="32"/>
+      <c r="P12" s="16"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>37</v>
+      </c>
+      <c r="O13" s="16"/>
+      <c r="P13" s="21"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Small bug fixes; refactor
</commit_message>
<xml_diff>
--- a/Wiring/RCCar Wiring.xlsx
+++ b/Wiring/RCCar Wiring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephhellerstein/home/Technical/Arduino/RCCar/Wiring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D12729-C870-6242-99D0-EF33AFC56F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCF0FC4-7F0D-2240-9F01-82E0CCA72017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="1140" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{0BE17797-1956-CB45-AFDB-7B911D2BE600}"/>
+    <workbookView xWindow="7800" yWindow="1140" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{0BE17797-1956-CB45-AFDB-7B911D2BE600}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1136,7 +1136,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1362,14 +1362,14 @@
         <v>35</v>
       </c>
       <c r="D13" s="2"/>
+      <c r="E13" s="12"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="12"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-      <c r="M13" s="12"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
+      <c r="P13" s="12"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
     </row>
@@ -1378,15 +1378,14 @@
         <v>36</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="13"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="H14" s="13"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
+      <c r="M14" s="13"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
-      <c r="P14" s="13"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
     </row>
@@ -1404,11 +1403,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700F51A8-449D-DA44-88E3-D7CBBE9512A0}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1716,18 +1715,16 @@
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
       <c r="D13" s="22"/>
-      <c r="E13" s="16"/>
+      <c r="E13" s="26"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="26"/>
       <c r="I13" s="22"/>
       <c r="J13" s="22"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
-      <c r="M13" s="26"/>
       <c r="N13" s="22"/>
       <c r="O13" s="22"/>
-      <c r="P13" s="16"/>
+      <c r="P13" s="26"/>
       <c r="Q13" s="22"/>
       <c r="R13" s="22"/>
     </row>
@@ -1738,18 +1735,16 @@
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
       <c r="D14" s="22"/>
-      <c r="E14" s="27"/>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="H14" s="27"/>
       <c r="I14" s="22"/>
       <c r="J14" s="22"/>
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
+      <c r="M14" s="27"/>
       <c r="N14" s="22"/>
       <c r="O14" s="22"/>
-      <c r="P14" s="27"/>
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
     </row>
@@ -1767,7 +1762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D2A009-778F-3F4C-8093-CF2587473A17}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>